<commit_message>
Moved model params to config file, added various debug comments, fixed error in temp converter
</commit_message>
<xml_diff>
--- a/TempSuitability_CSharp/calculate_max_tempsuitability.xlsx
+++ b/TempSuitability_CSharp/calculate_max_tempsuitability.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="4665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="4665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$K$2</definedName>
@@ -147,6 +148,1463 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1.0270692948112417</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0448357009900264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1191982856594138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79335738717055593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9422130996789303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96559189246688937</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97506365274116036</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.980167257186077</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9833392756813929</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98548646853577238</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98702328217933777</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98816581941101522</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98903760216826897</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98971414176315442</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9902439802008941</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99065951153138854</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99098292882195493</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9912296653057634</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99141046362218554</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99153265029719606</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99160092309363101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99161781961231532</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99158395831889201</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99149809598091698</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99135701168672286</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99115519678228459</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99088429313054727</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99053216725585924</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99008141478981193</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98950691735425023</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98877173327610934</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98781988354218375</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.98656295549767647</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.98485336662479239</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.98242576391080561</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.97875133936830383</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.97260447711634834</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9603542286201433</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.92439449833944864</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0772427440895893</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0368962583280865</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.023819754002911</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0173667086197453</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0135315946372074</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$1:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1.0234388176904146</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0358662890681127</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0738487782880253</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90086765942676705</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95559787967339516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97036358728766481</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97734856430020522</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98141146187397121</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98405321263555867</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98589379457027071</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98723626629271999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98824623925708277</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98902166455423446</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98962394464239944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9900932605037992</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99045671810453761</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99073293889470471</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99093476215441867</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99107088146717803</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.9911468424815677</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99116563103356081</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99112797376577988</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99103240956211014</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99087514521963482</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99064966806446986</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99034603892994666</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.98994971418497557</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.98943961537196712</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98878491757575004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98793952254712181</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98683207458803102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.98534673633361736</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.98328297124558661</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.98026159680598646</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.97546883063427448</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.96677570572706628</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.94613524387352377</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.78717347010442873</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0546130794066118</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0305415548363415</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.0209497863036756</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0157744634045485</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0125389393040167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="507740280"/>
+        <c:axId val="507740672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="507740280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507740672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="507740672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.95000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507740280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L373"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8672,4 +10130,656 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <f>POWER((EXP(-1 / (-4.4 + (1.31*A1) - (0.03 * (POWER(A1, 2)))))),(1/12))</f>
+        <v>1.0270692948112417</v>
+      </c>
+      <c r="C1">
+        <f xml:space="preserve"> POWER((1-( 1 / (-4.4 + 1.31 *A1 -0.03*(POWER(A1,2))))),(1/12))</f>
+        <v>1.0234388176904146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B45" si="0">POWER((EXP(-1 / (-4.4 + (1.31*A2) - (0.03 * (POWER(A2, 2)))))),(1/12))</f>
+        <v>1.0448357009900264</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C45" si="1" xml:space="preserve"> POWER((1-( 1 / (-4.4 + 1.31 *A2 -0.03*(POWER(A2,2))))),(1/12))</f>
+        <v>1.0358662890681127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>1.1191982856594138</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="1"/>
+        <v>1.0738487782880253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.79335738717055593</v>
+      </c>
+      <c r="C4" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.9422130996789303</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0.90086765942676705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.96559189246688937</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.95559787967339516</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.97506365274116036</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.97036358728766481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0.980167257186077</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.97734856430020522</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.9833392756813929</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.98141146187397121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.98548646853577238</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.98405321263555867</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.98702328217933777</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.98589379457027071</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0.98816581941101522</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.98723626629271999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0.98903760216826897</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.98824623925708277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0.98971414176315442</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.98902166455423446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.9902439802008941</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.98962394464239944</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.99065951153138854</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.9900932605037992</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.99098292882195493</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.99045671810453761</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.9912296653057634</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.99073293889470471</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.99141046362218554</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.99093476215441867</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.99153265029719606</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0.99107088146717803</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.99160092309363101</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0.9911468424815677</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0.99161781961231532</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0.99116563103356081</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.99158395831889201</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.99112797376577988</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.99149809598091698</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.99103240956211014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.99135701168672286</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0.99087514521963482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.99115519678228459</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.99064966806446986</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0.99088429313054727</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0.99034603892994666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0.99053216725585924</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0.98994971418497557</v>
+      </c>
+      <c r="D28">
+        <f>POWER(C28,(1/12))</f>
+        <v>0.99915859327331935</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0.99008141478981193</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>0.98943961537196712</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D39" si="2">POWER(C29,(1/12))</f>
+        <v>0.99911567947570756</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.98950691735425023</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>0.98878491757575004</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>0.9990605710685927</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0.98877173327610934</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>0.98793952254712181</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>0.99898936144743511</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0.98781988354218375</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>0.98683207458803102</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>0.99889599392867778</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0.98656295549767647</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0.98534673633361736</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>0.99877061604812989</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>0.98485336662479239</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>0.98328297124558661</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>0.99859612507978357</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0.98242576391080561</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0.98026159680598646</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>0.99834006193849989</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>0.97875133936830383</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0.97546883063427448</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>0.9979323844992195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>0.97260447711634834</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>0.96677570572706628</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>0.99718823053200878</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>0.9603542286201433</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0.94613524387352377</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>0.99539648246742474</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>0.92439449833944864</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>0.78717347010442873</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>0.98025531119753473</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C40" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>1.0772427440895893</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>1.0546130794066118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>1.0368962583280865</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>1.0305415548363415</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>1.023819754002911</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>1.0209497863036756</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>1.0173667086197453</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>1.0157744634045485</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>1.0135315946372074</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>1.0125389393040167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started adding code for reading humidity data
</commit_message>
<xml_diff>
--- a/TempSuitability_CSharp/calculate_max_tempsuitability.xlsx
+++ b/TempSuitability_CSharp/calculate_max_tempsuitability.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>surving_frac</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>Solve for max value of this cell by adjusting k2 using Solver</t>
+  </si>
+  <si>
+    <t>tempC</t>
+  </si>
+  <si>
+    <t>martens</t>
+  </si>
+  <si>
+    <t>gething</t>
+  </si>
+  <si>
+    <t>bayou_mordecai</t>
+  </si>
+  <si>
+    <t>martens_recal</t>
   </si>
 </sst>
 </file>
@@ -204,6 +219,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>martens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -230,7 +256,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$1:$A$45</c:f>
+              <c:f>Sheet2!$A$2:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
@@ -374,7 +400,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$1:$B$45</c:f>
+              <c:f>Sheet2!$B$2:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
@@ -521,6 +547,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gething</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -547,7 +584,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$1:$A$45</c:f>
+              <c:f>Sheet2!$A$2:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
@@ -691,7 +728,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$C$1:$C$45</c:f>
+              <c:f>Sheet2!$C$2:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
@@ -829,6 +866,374 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>1.0125389393040167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bayou_mordecai</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>0.95252828412793089</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95726501753558468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96154499761331591</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96542215770485085</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96894021058319868</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97213501507196376</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97503628588016511</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97766885361879474</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98005360945468134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98220822401343322</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98414770161832588</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98588481234673897</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98743043197399183</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98879381142326894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98998279147664869</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99100397436158449</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99186286085351927</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99256395936373765</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99311087186800151</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99350636030959549</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99375239616444533</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99385019510365036</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99380023806990525</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99360227955309754</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99325534337024302</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99275770579436939</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9921068654064602</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.991299498533601</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99033139855045516</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98919739661784001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9878912605566339</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98640556743341956</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.98473154396279616</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.98285886686261037</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.98077541261729606</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.97846694239138299</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.97591670260589647</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.97310491419713074</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.97000811264092768</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.96659828454351504</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.96284172182457517</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.95869747589582044</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.95411523237585183</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.94903232471282106</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.94336943034320764</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>martens_recal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1.0390127265136946</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7070920861939314</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95347764337027097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97672002409415193</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98413163203808407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98775758567613503</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98989383661962271</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99129050662114904</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99226523290279844</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99297540233260084</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99350770894717777</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99391365203481274</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99422555561590842</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99446452317408296</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99464468466741407</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99477559084701317</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99486361408765756</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99491278004674266</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99492524870980625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99490155790229617</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99484068230907641</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99473992040064885</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99459458535200296</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99439743130451119</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99413767586043666</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99379935120900398</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99335845904907083</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99277784754530096</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99199741853135304</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.99091387191711666</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98933418677928475</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98685223853873749</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.98244418637284914</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9725769283386293</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.93138580153553185</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1144905758757722</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0299221799787779</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.0168039446194543</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0114943976235469</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.0086291107741117</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0068411899765795</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0056224415184631</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.004740626075324</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0040745616943396</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0035548429980319</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -843,11 +1248,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="507740280"/>
-        <c:axId val="507740672"/>
+        <c:axId val="438442672"/>
+        <c:axId val="521262272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="507740280"/>
+        <c:axId val="438442672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,14 +1309,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507740672"/>
+        <c:crossAx val="521262272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="507740672"/>
+        <c:axId val="521262272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.05"/>
           <c:min val="0.95000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -967,7 +1373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507740280"/>
+        <c:crossAx val="438442672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -979,6 +1385,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1576,15 +2014,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1872,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L373"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10134,648 +10572,977 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1">
-        <f>POWER((EXP(-1 / (-4.4 + (1.31*A1) - (0.03 * (POWER(A1, 2)))))),(1/12))</f>
+      <c r="B2">
+        <f>POWER((EXP(-1 / (-4.4 + (1.31*A2) - (0.03 * (POWER(A2, 2)))))),(1/12))</f>
         <v>1.0270692948112417</v>
       </c>
-      <c r="C1">
-        <f xml:space="preserve"> POWER((1-( 1 / (-4.4 + 1.31 *A1 -0.03*(POWER(A1,2))))),(1/12))</f>
+      <c r="C2">
+        <f xml:space="preserve"> POWER((1-( 1 / (-4.4 + 1.31 *A2 -0.03*(POWER(A2,2))))),(1/12))</f>
         <v>1.0234388176904146</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D2">
+        <f>POWER((EXP(-1 / (-4.31564 + (2.19646*A2) - (0.058276 * (POWER(A2, 2)))))),(1/12))</f>
+        <v>1.0390127265136946</v>
+      </c>
+      <c r="E2">
+        <f>POWER((-0.000828*POWER(A2,2) + 0.0367*A2 +0.522),1/12)</f>
+        <v>0.95252828412793089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B2">
-        <f t="shared" ref="B2:B45" si="0">POWER((EXP(-1 / (-4.4 + (1.31*A2) - (0.03 * (POWER(A2, 2)))))),(1/12))</f>
+      <c r="B3">
+        <f t="shared" ref="B3:B46" si="0">POWER((EXP(-1 / (-4.4 + (1.31*A3) - (0.03 * (POWER(A3, 2)))))),(1/12))</f>
         <v>1.0448357009900264</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C45" si="1" xml:space="preserve"> POWER((1-( 1 / (-4.4 + 1.31 *A2 -0.03*(POWER(A2,2))))),(1/12))</f>
+      <c r="C3">
+        <f t="shared" ref="C3:C46" si="1" xml:space="preserve"> POWER((1-( 1 / (-4.4 + 1.31 *A3 -0.03*(POWER(A3,2))))),(1/12))</f>
         <v>1.0358662890681127</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D3">
+        <f t="shared" ref="D3:D46" si="2">POWER((EXP(-1 / (-4.31564 + (2.19646*A3) - (0.058276 * (POWER(A3, 2)))))),(1/12))</f>
+        <v>1.7070920861939314</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E46" si="3">POWER((-0.000828*POWER(A3,2) + 0.0367*A3 +0.522),1/12)</f>
+        <v>0.95726501753558468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <f t="shared" si="0"/>
         <v>1.1191982856594138</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <f t="shared" si="1"/>
         <v>1.0738487782880253</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>0.95347764337027097</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>0.96154499761331591</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>0.79335738717055593</v>
       </c>
-      <c r="C4" t="e">
+      <c r="C5" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>0.97672002409415193</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>0.96542215770485085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>0.9422130996789303</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <f t="shared" si="1"/>
         <v>0.90086765942676705</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.98413163203808407</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>0.96894021058319868</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>0.96559189246688937</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <f t="shared" si="1"/>
         <v>0.95559787967339516</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>0.98775758567613503</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>0.97213501507196376</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>0.97506365274116036</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <f t="shared" si="1"/>
         <v>0.97036358728766481</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>0.98989383661962271</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>0.97503628588016511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>0.980167257186077</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <f t="shared" si="1"/>
         <v>0.97734856430020522</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.99129050662114904</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>0.97766885361879474</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>0.9833392756813929</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f t="shared" si="1"/>
         <v>0.98141146187397121</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.99226523290279844</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>0.98005360945468134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>0.98548646853577238</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f t="shared" si="1"/>
         <v>0.98405321263555867</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0.99297540233260084</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>0.98220822401343322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <f t="shared" si="0"/>
         <v>0.98702328217933777</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <f t="shared" si="1"/>
         <v>0.98589379457027071</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>0.99350770894717777</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>0.98414770161832588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <f t="shared" si="0"/>
         <v>0.98816581941101522</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <f t="shared" si="1"/>
         <v>0.98723626629271999</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0.99391365203481274</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>0.98588481234673897</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <f t="shared" si="0"/>
         <v>0.98903760216826897</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <f t="shared" si="1"/>
         <v>0.98824623925708277</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>0.99422555561590842</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>0.98743043197399183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <f t="shared" si="0"/>
         <v>0.98971414176315442</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <f t="shared" si="1"/>
         <v>0.98902166455423446</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.99446452317408296</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>0.98879381142326894</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <f t="shared" si="0"/>
         <v>0.9902439802008941</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <f t="shared" si="1"/>
         <v>0.98962394464239944</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.99464468466741407</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>0.98998279147664869</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <f t="shared" si="0"/>
         <v>0.99065951153138854</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <f t="shared" si="1"/>
         <v>0.9900932605037992</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.99477559084701317</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>0.99100397436158449</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <f t="shared" si="0"/>
         <v>0.99098292882195493</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <f t="shared" si="1"/>
         <v>0.99045671810453761</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0.99486361408765756</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>0.99186286085351927</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <f t="shared" si="0"/>
         <v>0.9912296653057634</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <f t="shared" si="1"/>
         <v>0.99073293889470471</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>0.99491278004674266</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>0.99256395936373765</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <f t="shared" si="0"/>
         <v>0.99141046362218554</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <f t="shared" si="1"/>
         <v>0.99093476215441867</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>0.99492524870980625</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>0.99311087186800151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <f t="shared" si="0"/>
         <v>0.99153265029719606</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <f t="shared" si="1"/>
         <v>0.99107088146717803</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>0.99490155790229617</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>0.99350636030959549</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <f t="shared" si="0"/>
         <v>0.99160092309363101</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <f t="shared" si="1"/>
         <v>0.9911468424815677</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>0.99484068230907641</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>0.99375239616444533</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <f t="shared" si="0"/>
         <v>0.99161781961231532</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <f t="shared" si="1"/>
         <v>0.99116563103356081</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>0.99473992040064885</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>0.99385019510365036</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <f t="shared" si="0"/>
         <v>0.99158395831889201</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <f t="shared" si="1"/>
         <v>0.99112797376577988</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>0.99459458535200296</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>0.99380023806990525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f t="shared" si="0"/>
         <v>0.99149809598091698</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f t="shared" si="1"/>
         <v>0.99103240956211014</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>0.99439743130451119</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>0.99360227955309754</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <f t="shared" si="0"/>
         <v>0.99135701168672286</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f t="shared" si="1"/>
         <v>0.99087514521963482</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>0.99413767586043666</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>0.99325534337024302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>0.99115519678228459</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <f t="shared" si="1"/>
         <v>0.99064966806446986</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>0.99379935120900398</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>0.99275770579436939</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <f t="shared" si="0"/>
         <v>0.99088429313054727</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <f t="shared" si="1"/>
         <v>0.99034603892994666</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>0.99335845904907083</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>0.9921068654064602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <f t="shared" si="0"/>
         <v>0.99053216725585924</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <f t="shared" si="1"/>
         <v>0.98994971418497557</v>
       </c>
-      <c r="D28">
-        <f>POWER(C28,(1/12))</f>
-        <v>0.99915859327331935</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>0.99277784754530096</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>0.991299498533601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <f t="shared" si="0"/>
         <v>0.99008141478981193</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <f t="shared" si="1"/>
         <v>0.98943961537196712</v>
       </c>
-      <c r="D29">
-        <f t="shared" ref="D29:D39" si="2">POWER(C29,(1/12))</f>
-        <v>0.99911567947570756</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>0.99199741853135304</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>0.99033139855045516</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <f t="shared" si="0"/>
         <v>0.98950691735425023</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <f t="shared" si="1"/>
         <v>0.98878491757575004</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <f t="shared" si="2"/>
-        <v>0.9990605710685927</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+        <v>0.99091387191711666</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>0.98919739661784001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <f t="shared" si="0"/>
         <v>0.98877173327610934</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <f t="shared" si="1"/>
         <v>0.98793952254712181</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <f t="shared" si="2"/>
-        <v>0.99898936144743511</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+        <v>0.98933418677928475</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>0.9878912605566339</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <f t="shared" si="0"/>
         <v>0.98781988354218375</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <f t="shared" si="1"/>
         <v>0.98683207458803102</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <f t="shared" si="2"/>
-        <v>0.99889599392867778</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+        <v>0.98685223853873749</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>0.98640556743341956</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <f t="shared" si="0"/>
         <v>0.98656295549767647</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f t="shared" si="1"/>
         <v>0.98534673633361736</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <f t="shared" si="2"/>
-        <v>0.99877061604812989</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+        <v>0.98244418637284914</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>0.98473154396279616</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <f t="shared" si="0"/>
         <v>0.98485336662479239</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <f t="shared" si="1"/>
         <v>0.98328297124558661</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <f t="shared" si="2"/>
-        <v>0.99859612507978357</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+        <v>0.9725769283386293</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>0.98285886686261037</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <f t="shared" si="0"/>
         <v>0.98242576391080561</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f t="shared" si="1"/>
         <v>0.98026159680598646</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <f t="shared" si="2"/>
-        <v>0.99834006193849989</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+        <v>0.93138580153553185</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>0.98077541261729606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <f t="shared" si="0"/>
         <v>0.97875133936830383</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f t="shared" si="1"/>
         <v>0.97546883063427448</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <f t="shared" si="2"/>
-        <v>0.9979323844992195</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
+        <v>1.1144905758757722</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>0.97846694239138299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <f t="shared" si="0"/>
         <v>0.97260447711634834</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <f t="shared" si="1"/>
         <v>0.96677570572706628</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <f t="shared" si="2"/>
-        <v>0.99718823053200878</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
+        <v>1.0299221799787779</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>0.97591670260589647</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <f t="shared" si="0"/>
         <v>0.9603542286201433</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <f t="shared" si="1"/>
         <v>0.94613524387352377</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <f t="shared" si="2"/>
-        <v>0.99539648246742474</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
+        <v>1.0168039446194543</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>0.97310491419713074</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <f t="shared" si="0"/>
         <v>0.92439449833944864</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <f t="shared" si="1"/>
         <v>0.78717347010442873</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <f t="shared" si="2"/>
-        <v>0.98025531119753473</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
+        <v>1.0114943976235469</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>0.97000811264092768</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C40" t="e">
+      <c r="C41" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>1.0086291107741117</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>0.96659828454351504</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <f t="shared" si="0"/>
         <v>1.0772427440895893</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <f t="shared" si="1"/>
         <v>1.0546130794066118</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>1.0068411899765795</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>0.96284172182457517</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <f t="shared" si="0"/>
         <v>1.0368962583280865</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <f t="shared" si="1"/>
         <v>1.0305415548363415</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>1.0056224415184631</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="3"/>
+        <v>0.95869747589582044</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <f t="shared" si="0"/>
         <v>1.023819754002911</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <f t="shared" si="1"/>
         <v>1.0209497863036756</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>1.004740626075324</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>0.95411523237585183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <f t="shared" si="0"/>
         <v>1.0173667086197453</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <f t="shared" si="1"/>
         <v>1.0157744634045485</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>1.0040745616943396</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>0.94903232471282106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <f t="shared" si="0"/>
         <v>1.0135315946372074</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <f t="shared" si="1"/>
         <v>1.0125389393040167</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>1.0035548429980319</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="3"/>
+        <v>0.94336943034320764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>